<commit_message>
#9 in general for main data descriptor and #8
</commit_message>
<xml_diff>
--- a/output/soil.xlsx
+++ b/output/soil.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="90">
   <si>
     <t>Location</t>
   </si>
@@ -600,40 +600,40 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" t="s">
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -641,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -656,16 +656,16 @@
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
         <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s">
         <v>30</v>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -694,7 +694,7 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
         <v>59</v>
@@ -703,7 +703,7 @@
         <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
         <v>30</v>
@@ -717,10 +717,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -732,22 +732,22 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
         <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -755,7 +755,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -770,16 +770,16 @@
         <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K12" t="s">
         <v>86</v>
@@ -790,40 +790,40 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="L13" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -831,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -843,25 +843,25 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" t="s">
         <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
         <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15">
@@ -869,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -884,16 +884,16 @@
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
         <v>30</v>
@@ -904,40 +904,40 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
         <v>30</v>
       </c>
       <c r="L16" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -945,22 +945,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H17" t="s">
         <v>56</v>
@@ -969,7 +969,7 @@
         <v>71</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" t="s">
         <v>30</v>
@@ -983,19 +983,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
         <v>51</v>
@@ -1010,7 +1010,7 @@
         <v>83</v>
       </c>
       <c r="K18" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="L18" t="s">
         <v>30</v>
@@ -1021,7 +1021,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
@@ -1059,31 +1059,31 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
         <v>56</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
         <v>85</v>
@@ -1094,40 +1094,40 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="L21" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
@@ -1135,7 +1135,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -1173,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -1208,13 +1208,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -1226,22 +1226,22 @@
         <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I24" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="J24" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="K24" t="s">
         <v>30</v>
       </c>
       <c r="L24" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25">
@@ -1249,36 +1249,112 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
         <v>19</v>
       </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>